<commit_message>
10v10 USQ 11 Cup games Pt. 2
</commit_message>
<xml_diff>
--- a/10v10/11/USQ-Cup/TEXAS_TXST.xlsx
+++ b/10v10/11/USQ-Cup/TEXAS_TXST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghu\quidditch\live-stats\11\USQCup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghu\quidditch\10v10\11\USQ-Cup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CB77B7-E95C-401C-BE8B-2641B2A4B19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C262187-743F-4EC9-BAFE-BE55D32457A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="140">
   <si>
     <t>A</t>
   </si>
@@ -56,9 +58,6 @@
   </si>
   <si>
     <t>GP</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>TC</t>
@@ -172,12 +171,6 @@
     <t>33,19</t>
   </si>
   <si>
-    <t>EP</t>
-  </si>
-  <si>
-    <t>ET</t>
-  </si>
-  <si>
     <t>2,11</t>
   </si>
   <si>
@@ -205,9 +198,6 @@
     <t>TIM NGUYEN</t>
   </si>
   <si>
-    <t>2YB23</t>
-  </si>
-  <si>
     <t>R17</t>
   </si>
   <si>
@@ -232,7 +222,235 @@
     <t>OMAR GARZA</t>
   </si>
   <si>
-    <t>R15</t>
+    <t>0013</t>
+  </si>
+  <si>
+    <t>0058</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>0124</t>
+  </si>
+  <si>
+    <t>0206</t>
+  </si>
+  <si>
+    <t>0238</t>
+  </si>
+  <si>
+    <t>0329</t>
+  </si>
+  <si>
+    <t>0356</t>
+  </si>
+  <si>
+    <t>0400</t>
+  </si>
+  <si>
+    <t>0429</t>
+  </si>
+  <si>
+    <t>0454</t>
+  </si>
+  <si>
+    <t>0501</t>
+  </si>
+  <si>
+    <t>0541</t>
+  </si>
+  <si>
+    <t>0610</t>
+  </si>
+  <si>
+    <t>0639</t>
+  </si>
+  <si>
+    <t>0707</t>
+  </si>
+  <si>
+    <t>0733</t>
+  </si>
+  <si>
+    <t>0807</t>
+  </si>
+  <si>
+    <t>0903</t>
+  </si>
+  <si>
+    <t>0908</t>
+  </si>
+  <si>
+    <t>0928</t>
+  </si>
+  <si>
+    <t>0955</t>
+  </si>
+  <si>
+    <t>1023</t>
+  </si>
+  <si>
+    <t>1048</t>
+  </si>
+  <si>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>1154</t>
+  </si>
+  <si>
+    <t>1216</t>
+  </si>
+  <si>
+    <t>1223</t>
+  </si>
+  <si>
+    <t>1236</t>
+  </si>
+  <si>
+    <t>1301</t>
+  </si>
+  <si>
+    <t>1354</t>
+  </si>
+  <si>
+    <t>1437</t>
+  </si>
+  <si>
+    <t>1453</t>
+  </si>
+  <si>
+    <t>1534</t>
+  </si>
+  <si>
+    <t>1618</t>
+  </si>
+  <si>
+    <t>1647</t>
+  </si>
+  <si>
+    <t>1657</t>
+  </si>
+  <si>
+    <t>1703</t>
+  </si>
+  <si>
+    <t>1756</t>
+  </si>
+  <si>
+    <t>1825</t>
+  </si>
+  <si>
+    <t>1851</t>
+  </si>
+  <si>
+    <t>1915</t>
+  </si>
+  <si>
+    <t>1935</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2048</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>2209</t>
+  </si>
+  <si>
+    <t>2215</t>
+  </si>
+  <si>
+    <t>2312</t>
+  </si>
+  <si>
+    <t>2329</t>
+  </si>
+  <si>
+    <t>2410</t>
+  </si>
+  <si>
+    <t>2429</t>
+  </si>
+  <si>
+    <t>2517</t>
+  </si>
+  <si>
+    <t>2519</t>
+  </si>
+  <si>
+    <t>2643</t>
+  </si>
+  <si>
+    <t>2717</t>
+  </si>
+  <si>
+    <t>2801</t>
+  </si>
+  <si>
+    <t>2847</t>
+  </si>
+  <si>
+    <t>R71</t>
+  </si>
+  <si>
+    <t>2929</t>
+  </si>
+  <si>
+    <t>3016</t>
+  </si>
+  <si>
+    <t>3106</t>
+  </si>
+  <si>
+    <t>3124</t>
+  </si>
+  <si>
+    <t>3157</t>
+  </si>
+  <si>
+    <t>3322</t>
+  </si>
+  <si>
+    <t>3248</t>
+  </si>
+  <si>
+    <t>3256</t>
+  </si>
+  <si>
+    <t>YB2,2YB23</t>
+  </si>
+  <si>
+    <t>3432</t>
+  </si>
+  <si>
+    <t>3453</t>
+  </si>
+  <si>
+    <t>3549</t>
+  </si>
+  <si>
+    <t>3602</t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>3702</t>
+  </si>
+  <si>
+    <t>3721</t>
+  </si>
+  <si>
+    <t>3847</t>
   </si>
 </sst>
 </file>
@@ -518,7 +736,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -526,20 +752,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,8 +979,8 @@
   </sheetPr>
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:W5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="77" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -791,21 +1009,21 @@
     <row r="1" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
       <c r="R1" s="2"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -818,142 +1036,142 @@
     </row>
     <row r="2" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="25">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="21">
         <f>COUNTIFS(A:A,"G*") + COUNTIFS(G:G,"G*")+COUNTIFS(M:M,"G*")+COUNTIFS(S:S,"G*")</f>
         <v>19</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="26" t="str">
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="27" t="str">
         <f>IF(COUNTIF($A$7:$X$59,"RCA"),"*","")&amp;IF(COUNTIF($A$7:$X$59,"OCA"),"^","")&amp;IF(COUNTIF($R$7:$X$59,"2CA"),"!","")</f>
         <v>*</v>
       </c>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="17" t="str">
+      <c r="P2" s="22"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="28" t="str">
         <f>CONCATENATE(LEN(O2)*30+L2*10,O2)</f>
         <v>220*</v>
       </c>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="19"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="22"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="26"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="25">
+      <c r="C4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="22"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="21">
         <f>COUNTIFS(D:D,"G*")+COUNTIFS(J:J,"G*")+COUNTIFS(P:P,"G*")+COUNTIFS(V:V,"G*")</f>
         <v>14</v>
       </c>
-      <c r="M4" s="18"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="26" t="str">
+      <c r="M4" s="22"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="27" t="str">
         <f>IF(COUNTIF($A$7:$R$59,"RCB"),"*","")&amp;IF(COUNTIF($A$7:$R$59,"OCB"),"^","")&amp;IF(COUNTIF($A$7:$R$59,"2CB"),"!","")</f>
         <v/>
       </c>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="17" t="str">
+      <c r="P4" s="22"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="28" t="str">
         <f>CONCATENATE(LEN(O4)*30+L4*10,O4)</f>
         <v>140</v>
       </c>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="19"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="23"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="22"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="26"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -996,41 +1214,55 @@
       <c r="E7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R7" s="8"/>
+      <c r="R7" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="S7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U7" s="5"/>
+      <c r="U7" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="V7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X7" s="8"/>
+      <c r="X7" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
@@ -1129,44 +1361,58 @@
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="M10" s="3"/>
       <c r="N10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="O10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="P10" s="6"/>
       <c r="Q10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R10" s="8"/>
+      <c r="R10" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="S10" s="3"/>
       <c r="T10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U10" s="5"/>
+      <c r="U10" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="V10" s="6"/>
       <c r="W10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X10" s="8"/>
+      <c r="X10" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
@@ -1178,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>8</v>
@@ -1215,7 +1461,7 @@
         <v>33</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q11" s="10">
         <v>9</v>
@@ -1275,42 +1521,58 @@
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R13" s="8"/>
+      <c r="R13" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="S13" s="3"/>
       <c r="T13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U13" s="5"/>
+      <c r="U13" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="V13" s="6"/>
       <c r="W13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X13" s="8"/>
+      <c r="X13" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
@@ -1419,42 +1681,58 @@
       <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="J16" s="6"/>
       <c r="K16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O16" s="5"/>
+      <c r="O16" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R16" s="8"/>
+      <c r="R16" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="S16" s="3"/>
       <c r="T16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U16" s="5"/>
+      <c r="U16" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="V16" s="6"/>
       <c r="W16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X16" s="8"/>
+      <c r="X16" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
@@ -1463,7 +1741,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="10">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="9" t="s">
@@ -1472,8 +1750,8 @@
       <c r="E17" s="10">
         <v>7</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>9</v>
+      <c r="F17" s="11">
+        <v>21</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>5</v>
@@ -1558,47 +1836,63 @@
     </row>
     <row r="19" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O19" s="5"/>
+      <c r="O19" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R19" s="8"/>
+      <c r="R19" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="S19" s="3"/>
       <c r="T19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U19" s="5"/>
+      <c r="U19" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="V19" s="6"/>
       <c r="W19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X19" s="8"/>
+      <c r="X19" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
@@ -1628,7 +1922,7 @@
         <v>6</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>3</v>
@@ -1637,7 +1931,7 @@
         <v>12</v>
       </c>
       <c r="L20" s="11">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M20" s="9" t="s">
         <v>7</v>
@@ -1646,10 +1940,10 @@
         <v>6</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q20" s="10">
         <v>8</v>
@@ -1704,47 +1998,63 @@
     </row>
     <row r="22" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="5"/>
+      <c r="I22" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="J22" s="6"/>
       <c r="K22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L22" s="8"/>
+      <c r="L22" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="M22" s="3"/>
       <c r="N22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O22" s="5"/>
+      <c r="O22" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R22" s="8"/>
+      <c r="R22" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="S22" s="3"/>
       <c r="T22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U22" s="5"/>
+      <c r="U22" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="V22" s="6"/>
       <c r="W22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X22" s="8"/>
+      <c r="X22" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
@@ -1759,7 +2069,7 @@
         <v>33</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="10">
         <v>33</v>
@@ -1768,7 +2078,7 @@
         <v>50</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H23" s="10">
         <v>6</v>
@@ -1777,16 +2087,16 @@
         <v>19</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K23" s="10">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="L23" s="11">
         <v>1</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N23" s="10">
         <v>19</v>
@@ -1795,7 +2105,7 @@
         <v>9</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q23" s="10">
         <v>41</v>
@@ -1804,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="S23" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T23" s="10">
         <v>2</v>
@@ -1857,57 +2167,75 @@
       <c r="B25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="G25" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I25" s="5"/>
+      <c r="I25" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="J25" s="6"/>
       <c r="K25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L25" s="8"/>
+      <c r="L25" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="M25" s="3"/>
       <c r="N25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O25" s="5"/>
+      <c r="O25" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R25" s="8"/>
+      <c r="R25" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="S25" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="T25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U25" s="5"/>
+      <c r="U25" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="V25" s="6"/>
       <c r="W25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X25" s="8"/>
+      <c r="X25" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B26" s="10">
+        <v>23</v>
+      </c>
+      <c r="C26" s="11">
         <v>41</v>
       </c>
-      <c r="C26" s="11"/>
       <c r="D26" s="9" t="s">
         <v>7</v>
       </c>
@@ -1915,7 +2243,7 @@
         <v>19</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>5</v>
@@ -1925,7 +2253,7 @@
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K26" s="10">
         <v>9</v>
@@ -1934,7 +2262,7 @@
         <v>6</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N26" s="10">
         <v>1</v>
@@ -1958,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="V26" s="9" t="s">
         <v>5</v>
@@ -1999,50 +2327,70 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="J28" s="6"/>
       <c r="K28" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="3"/>
+      <c r="L28" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="N28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O28" s="5"/>
+      <c r="O28" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="P28" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q28" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R28" s="8"/>
+      <c r="R28" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="S28" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U28" s="5"/>
+      <c r="U28" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="V28" s="6"/>
       <c r="W28" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X28" s="8"/>
+      <c r="X28" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
@@ -2057,14 +2405,12 @@
         <v>3</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E29" s="10">
         <v>1</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>9</v>
-      </c>
+      <c r="F29" s="11"/>
       <c r="G29" s="9" t="s">
         <v>7</v>
       </c>
@@ -2072,10 +2418,10 @@
         <v>69</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K29" s="10">
         <v>9</v>
@@ -2093,7 +2439,7 @@
         <v>3</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q29" s="10">
         <v>24</v>
@@ -2152,49 +2498,65 @@
     </row>
     <row r="31" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="D31" s="6"/>
       <c r="E31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="8"/>
+      <c r="F31" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="G31" s="3"/>
       <c r="H31" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I31" s="5"/>
+      <c r="I31" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="J31" s="6"/>
       <c r="K31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L31" s="8"/>
+      <c r="L31" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="M31" s="3" t="s">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O31" s="5"/>
+      <c r="O31" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R31" s="8"/>
+      <c r="R31" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="S31" s="3"/>
       <c r="T31" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U31" s="5"/>
+      <c r="U31" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="V31" s="6"/>
       <c r="W31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X31" s="8"/>
+      <c r="X31" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
@@ -2216,7 +2578,7 @@
         <v>21</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H32" s="10">
         <v>21</v>
@@ -2264,8 +2626,8 @@
       <c r="W32" s="10">
         <v>8</v>
       </c>
-      <c r="X32" s="11">
-        <v>6</v>
+      <c r="X32" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
@@ -2300,22 +2662,28 @@
     </row>
     <row r="34" spans="1:26" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="D34" s="6"/>
       <c r="E34" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="8"/>
+      <c r="F34" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="G34" s="3"/>
       <c r="H34" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I34" s="5"/>
+      <c r="I34" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="J34" s="6"/>
       <c r="K34" s="7" t="s">
         <v>2</v>
@@ -2352,7 +2720,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>6</v>
@@ -2364,7 +2732,7 @@
         <v>2</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H35" s="10">
         <v>23</v>
@@ -29242,6 +29610,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R2:W3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:H5"/>
+    <mergeCell ref="I4:K5"/>
+    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="R4:W5"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
@@ -29251,13 +29626,6 @@
     <mergeCell ref="I2:K3"/>
     <mergeCell ref="L2:N3"/>
     <mergeCell ref="O2:Q3"/>
-    <mergeCell ref="R2:W3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:H5"/>
-    <mergeCell ref="I4:K5"/>
-    <mergeCell ref="L4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="R4:W5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -29301,7 +29669,7 @@
       </c>
       <c r="B3" s="16"/>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29310,7 +29678,7 @@
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29318,7 +29686,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="12"/>
     </row>
@@ -29340,7 +29708,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29348,10 +29716,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29359,7 +29727,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="12"/>
     </row>
@@ -29368,7 +29736,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="12"/>
     </row>
@@ -29378,7 +29746,7 @@
       </c>
       <c r="B12" s="16"/>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29387,7 +29755,7 @@
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29395,7 +29763,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="12"/>
     </row>
@@ -29411,7 +29779,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C16" s="12"/>
     </row>
@@ -29420,7 +29788,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="12"/>
     </row>
@@ -29435,10 +29803,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29453,7 +29821,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="12"/>
     </row>
@@ -29462,10 +29830,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29474,7 +29842,7 @@
       </c>
       <c r="B23" s="16"/>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29482,10 +29850,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29493,10 +29861,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29504,7 +29872,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="12"/>
     </row>
@@ -29525,7 +29893,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="12"/>
     </row>
@@ -29565,7 +29933,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="12"/>
     </row>
@@ -29616,7 +29984,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29674,7 +30042,7 @@
       </c>
       <c r="B52" s="16"/>
       <c r="C52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29700,7 +30068,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29757,7 +30125,7 @@
       </c>
       <c r="B65" s="16"/>
       <c r="C65" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29796,7 +30164,7 @@
       </c>
       <c r="B71" s="16"/>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29865,7 +30233,7 @@
       </c>
       <c r="B82" s="16"/>
       <c r="C82" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">

</xml_diff>